<commit_message>
update impor data anggota + simpanan
</commit_message>
<xml_diff>
--- a/public/template/template_anggota.xlsx
+++ b/public/template/template_anggota.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp8.2.0\htdocs\SIKOPDIT\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\SIKOPDIT\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5BE1CC-2715-4273-897E-568393D7ED6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="345" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nama</t>
   </si>
@@ -57,25 +56,37 @@
     <t>Sapon</t>
   </si>
   <si>
-    <t>Jl. Merdeka No. 1</t>
-  </si>
-  <si>
     <t>Petani</t>
   </si>
   <si>
     <t>Aktif</t>
   </si>
   <si>
-    <t>Andi Saputra Dhika</t>
-  </si>
-  <si>
-    <t>Siti Aisyah Titi</t>
+    <t>Saldo_sw</t>
+  </si>
+  <si>
+    <t>Saldo_swp</t>
+  </si>
+  <si>
+    <t>Saldo_sp</t>
+  </si>
+  <si>
+    <t>Saldo_ss</t>
+  </si>
+  <si>
+    <t>Hasan wisnu</t>
+  </si>
+  <si>
+    <t>Aisyah tithi</t>
+  </si>
+  <si>
+    <t>jl, merdeka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -132,6 +143,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,24 +426,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H14" sqref="H13:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,38 +474,74 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4">
         <v>1234567890123450</v>
       </c>
       <c r="C2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="3">
         <v>33003</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>50000</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>10000</v>
+      </c>
+      <c r="M2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>